<commit_message>
added contextual variables from census
</commit_message>
<xml_diff>
--- a/data/raw/contextual/formatted vars.xlsx
+++ b/data/raw/contextual/formatted vars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\personal projs\tax-yale\data\raw\contextual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2133084-4D03-4E5D-87AB-90BC8F7193C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001A6998-59F5-460B-B8C1-6454D38DF13E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variable descriptions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="270">
   <si>
     <t>name</t>
   </si>
@@ -151,63 +151,6 @@
     <t>B07004I_002</t>
   </si>
   <si>
-    <t>B19113_001</t>
-  </si>
-  <si>
-    <t>Estimate!!Median family income in the past 12 months (in 2018 inflation-adjusted dollars)</t>
-  </si>
-  <si>
-    <t>MEDIAN FAMILY INCOME IN THE PAST 12 MONTHS (IN 2018 INFLATION-ADJUSTED DOLLARS)</t>
-  </si>
-  <si>
-    <t>B19113B_001</t>
-  </si>
-  <si>
-    <t>MEDIAN FAMILY INCOME IN THE PAST 12 MONTHS (IN 2018 INFLATION-ADJUSTED DOLLARS) (BLACK OR AFRICAN AMERICAN ALONE HOUSEHOLDER)</t>
-  </si>
-  <si>
-    <t>B19113C_001</t>
-  </si>
-  <si>
-    <t>MEDIAN FAMILY INCOME IN THE PAST 12 MONTHS (IN 2018 INFLATION-ADJUSTED DOLLARS) (AMERICAN INDIAN AND ALASKA NATIVE ALONE HOUSEHOLDER)</t>
-  </si>
-  <si>
-    <t>B19113D_001</t>
-  </si>
-  <si>
-    <t>MEDIAN FAMILY INCOME IN THE PAST 12 MONTHS (IN 2018 INFLATION-ADJUSTED DOLLARS) (ASIAN ALONE HOUSEHOLDER)</t>
-  </si>
-  <si>
-    <t>B19113E_001</t>
-  </si>
-  <si>
-    <t>MEDIAN FAMILY INCOME IN THE PAST 12 MONTHS (IN 2018 INFLATION-ADJUSTED DOLLARS) (NATIVE HAWAIIAN AND OTHER PACIFIC ISLANDER ALONE HOUSEHOLDER)</t>
-  </si>
-  <si>
-    <t>B19113F_001</t>
-  </si>
-  <si>
-    <t>MEDIAN FAMILY INCOME IN THE PAST 12 MONTHS (IN 2018 INFLATION-ADJUSTED DOLLARS) (SOME OTHER RACE ALONE HOUSEHOLDER)</t>
-  </si>
-  <si>
-    <t>B19113G_001</t>
-  </si>
-  <si>
-    <t>MEDIAN FAMILY INCOME IN THE PAST 12 MONTHS (IN 2018 INFLATION-ADJUSTED DOLLARS) (TWO OR MORE RACES)</t>
-  </si>
-  <si>
-    <t>B19113H_001</t>
-  </si>
-  <si>
-    <t>MEDIAN FAMILY INCOME IN THE PAST 12 MONTHS (IN 2018 INFLATION-ADJUSTED DOLLARS) (WHITE ALONE, NOT HISPANIC OR LATINO HOUSEHOLDER)</t>
-  </si>
-  <si>
-    <t>B19113I_001</t>
-  </si>
-  <si>
-    <t>MEDIAN FAMILY INCOME IN THE PAST 12 MONTHS (IN 2018 INFLATION-ADJUSTED DOLLARS) (HISPANIC OR LATINO HOUSEHOLDER)</t>
-  </si>
-  <si>
     <t>B25003_001</t>
   </si>
   <si>
@@ -292,162 +235,108 @@
     <t>B25003I_003</t>
   </si>
   <si>
-    <t>Estimate!!Total!!Male!!High school graduate (includes equivalency)</t>
-  </si>
-  <si>
     <t>Estimate!!Total!!Male!!Bachelor's degree or higher</t>
   </si>
   <si>
     <t>Estimate!!Total!!Female</t>
   </si>
   <si>
-    <t>Estimate!!Total!!Female!!High school graduate (includes equivalency)</t>
-  </si>
-  <si>
     <t>Estimate!!Total!!Female!!Bachelor's degree or higher</t>
   </si>
   <si>
     <t>SEX BY EDUCATIONAL ATTAINMENT FOR THE POPULATION 25 YEARS AND OVER (BLACK OR AFRICAN AMERICAN ALONE)</t>
   </si>
   <si>
-    <t>C15002B_004</t>
-  </si>
-  <si>
     <t>C15002B_006</t>
   </si>
   <si>
     <t>C15002B_007</t>
   </si>
   <si>
-    <t>C15002B_009</t>
-  </si>
-  <si>
     <t>C15002B_011</t>
   </si>
   <si>
     <t>SEX BY EDUCATIONAL ATTAINMENT FOR THE POPULATION 25 YEARS AND OVER (AMERICAN INDIAN AND ALASKA NATIVE ALONE)</t>
   </si>
   <si>
-    <t>C15002C_004</t>
-  </si>
-  <si>
     <t>C15002C_006</t>
   </si>
   <si>
     <t>C15002C_007</t>
   </si>
   <si>
-    <t>C15002C_009</t>
-  </si>
-  <si>
     <t>C15002C_011</t>
   </si>
   <si>
     <t>SEX BY EDUCATIONAL ATTAINMENT FOR THE POPULATION 25 YEARS AND OVER (ASIAN ALONE)</t>
   </si>
   <si>
-    <t>C15002D_004</t>
-  </si>
-  <si>
     <t>C15002D_006</t>
   </si>
   <si>
     <t>C15002D_007</t>
   </si>
   <si>
-    <t>C15002D_009</t>
-  </si>
-  <si>
     <t>C15002D_011</t>
   </si>
   <si>
     <t>SEX BY EDUCATIONAL ATTAINMENT FOR THE POPULATION 25 YEARS AND OVER (NATIVE HAWAIIAN AND OTHER PACIFIC ISLANDER ALONE)</t>
   </si>
   <si>
-    <t>C15002E_004</t>
-  </si>
-  <si>
     <t>C15002E_006</t>
   </si>
   <si>
     <t>C15002E_007</t>
   </si>
   <si>
-    <t>C15002E_009</t>
-  </si>
-  <si>
     <t>C15002E_011</t>
   </si>
   <si>
     <t>SEX BY EDUCATIONAL ATTAINMENT FOR THE POPULATION 25 YEARS AND OVER (SOME OTHER RACE ALONE)</t>
   </si>
   <si>
-    <t>C15002F_004</t>
-  </si>
-  <si>
     <t>C15002F_006</t>
   </si>
   <si>
     <t>C15002F_007</t>
   </si>
   <si>
-    <t>C15002F_009</t>
-  </si>
-  <si>
     <t>C15002F_011</t>
   </si>
   <si>
     <t>SEX BY EDUCATIONAL ATTAINMENT FOR THE POPULATION 25 YEARS AND OVER (TWO OR MORE RACES)</t>
   </si>
   <si>
-    <t>C15002G_004</t>
-  </si>
-  <si>
     <t>C15002G_006</t>
   </si>
   <si>
     <t>C15002G_007</t>
   </si>
   <si>
-    <t>C15002G_009</t>
-  </si>
-  <si>
     <t>C15002G_011</t>
   </si>
   <si>
     <t>SEX BY EDUCATIONAL ATTAINMENT FOR THE POPULATION 25 YEARS AND OVER (WHITE ALONE, NOT HISPANIC OR LATINO)</t>
   </si>
   <si>
-    <t>C15002H_004</t>
-  </si>
-  <si>
     <t>C15002H_006</t>
   </si>
   <si>
     <t>C15002H_007</t>
   </si>
   <si>
-    <t>C15002H_009</t>
-  </si>
-  <si>
     <t>C15002H_011</t>
   </si>
   <si>
     <t>SEX BY EDUCATIONAL ATTAINMENT FOR THE POPULATION 25 YEARS AND OVER (HISPANIC OR LATINO)</t>
   </si>
   <si>
-    <t>C15002I_004</t>
-  </si>
-  <si>
     <t>C15002I_006</t>
   </si>
   <si>
     <t>C15002I_007</t>
   </si>
   <si>
-    <t>C15002I_009</t>
-  </si>
-  <si>
     <t>C15002I_011</t>
   </si>
   <si>
@@ -812,6 +701,135 @@
   </si>
   <si>
     <t>C27001B_006</t>
+  </si>
+  <si>
+    <t>B17020B_001</t>
+  </si>
+  <si>
+    <t>POVERTY STATUS IN THE PAST 12 MONTHS BY AGE (BLACK OR AFRICAN AMERICAN ALONE)</t>
+  </si>
+  <si>
+    <t>B17020B_002</t>
+  </si>
+  <si>
+    <t>Estimate!!Total!!Income in the past 12 months below poverty level</t>
+  </si>
+  <si>
+    <t>B17020C_001</t>
+  </si>
+  <si>
+    <t>POVERTY STATUS IN THE PAST 12 MONTHS BY AGE (AMERICAN INDIAN AND ALASKA NATIVE ALONE)</t>
+  </si>
+  <si>
+    <t>B17020C_002</t>
+  </si>
+  <si>
+    <t>B17020D_001</t>
+  </si>
+  <si>
+    <t>POVERTY STATUS IN THE PAST 12 MONTHS BY AGE (ASIAN ALONE)</t>
+  </si>
+  <si>
+    <t>B17020D_002</t>
+  </si>
+  <si>
+    <t>B17020E_001</t>
+  </si>
+  <si>
+    <t>POVERTY STATUS IN THE PAST 12 MONTHS BY AGE (NATIVE HAWAIIAN AND OTHER PACIFIC ISLANDER ALONE)</t>
+  </si>
+  <si>
+    <t>B17020E_002</t>
+  </si>
+  <si>
+    <t>B17020F_001</t>
+  </si>
+  <si>
+    <t>POVERTY STATUS IN THE PAST 12 MONTHS BY AGE (SOME OTHER RACE ALONE)</t>
+  </si>
+  <si>
+    <t>B17020F_002</t>
+  </si>
+  <si>
+    <t>B17020G_001</t>
+  </si>
+  <si>
+    <t>POVERTY STATUS IN THE PAST 12 MONTHS BY AGE (TWO OR MORE RACES)</t>
+  </si>
+  <si>
+    <t>B17020G_002</t>
+  </si>
+  <si>
+    <t>B17020H_001</t>
+  </si>
+  <si>
+    <t>POVERTY STATUS IN THE PAST 12 MONTHS BY AGE (WHITE ALONE, NOT HISPANIC OR LATINO)</t>
+  </si>
+  <si>
+    <t>B17020H_002</t>
+  </si>
+  <si>
+    <t>B17020I_001</t>
+  </si>
+  <si>
+    <t>POVERTY STATUS IN THE PAST 12 MONTHS BY AGE (HISPANIC OR LATINO)</t>
+  </si>
+  <si>
+    <t>B17020I_002</t>
+  </si>
+  <si>
+    <t>Estimate!!Total!!Male!!Less than high school diploma</t>
+  </si>
+  <si>
+    <t>Estimate!!Total!!Female!!Less than high school diploma</t>
+  </si>
+  <si>
+    <t>C15002B_003</t>
+  </si>
+  <si>
+    <t>C15002B_008</t>
+  </si>
+  <si>
+    <t>C15002C_003</t>
+  </si>
+  <si>
+    <t>C15002C_008</t>
+  </si>
+  <si>
+    <t>C15002D_003</t>
+  </si>
+  <si>
+    <t>C15002D_008</t>
+  </si>
+  <si>
+    <t>C15002E_003</t>
+  </si>
+  <si>
+    <t>C15002E_008</t>
+  </si>
+  <si>
+    <t>C15002F_003</t>
+  </si>
+  <si>
+    <t>C15002F_008</t>
+  </si>
+  <si>
+    <t>C15002G_003</t>
+  </si>
+  <si>
+    <t>C15002G_008</t>
+  </si>
+  <si>
+    <t>C15002H_003</t>
+  </si>
+  <si>
+    <t>C15002H_008</t>
+  </si>
+  <si>
+    <t>C15002I_003</t>
+  </si>
+  <si>
+    <t>C15002I_008</t>
   </si>
 </sst>
 </file>
@@ -1652,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D181"/>
+  <dimension ref="A1:D188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="D151" sqref="D151"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61:D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1666,7 +1684,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>234</v>
+        <v>197</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1680,7 +1698,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1694,7 +1712,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1708,7 +1726,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1722,7 +1740,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1736,7 +1754,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -1750,7 +1768,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -1764,7 +1782,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -1778,35 +1796,35 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="B9" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="C9" t="s">
-        <v>247</v>
+        <v>210</v>
       </c>
       <c r="D9" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>206</v>
       </c>
       <c r="C10" t="s">
-        <v>244</v>
+        <v>207</v>
       </c>
       <c r="D10" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1820,7 +1838,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -1834,7 +1852,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -1848,7 +1866,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -1862,7 +1880,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
@@ -1876,7 +1894,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="B16" t="s">
         <v>27</v>
@@ -1890,7 +1908,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
@@ -1904,7 +1922,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
@@ -1918,7 +1936,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
@@ -1932,7 +1950,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="B20" t="s">
         <v>33</v>
@@ -1946,7 +1964,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -1960,7 +1978,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
@@ -1974,7 +1992,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="B23" t="s">
         <v>37</v>
@@ -1988,7 +2006,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="B24" t="s">
         <v>39</v>
@@ -2002,7 +2020,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
@@ -2016,7 +2034,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="B26" t="s">
         <v>42</v>
@@ -2030,2172 +2048,2270 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>227</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>229</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>230</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>231</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>49</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>233</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>230</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>234</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>242</v>
+        <v>200</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>236</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>230</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>204</v>
+      </c>
+      <c r="B33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
         <v>238</v>
-      </c>
-      <c r="B33" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>239</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>230</v>
       </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>248</v>
+        <v>205</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>240</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>61</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>242</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>241</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>243</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>63</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>239</v>
+        <v>201</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>245</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="D38" t="s">
-        <v>67</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>239</v>
+        <v>199</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>246</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>67</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>240</v>
+        <v>199</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>248</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="D40" t="s">
-        <v>70</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>249</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>70</v>
+        <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>237</v>
+        <v>211</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>251</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D44" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>241</v>
+        <v>202</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>242</v>
+        <v>202</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>242</v>
+        <v>203</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>238</v>
+        <v>200</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>236</v>
+        <v>200</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D50" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>248</v>
+        <v>204</v>
       </c>
       <c r="B52" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D52" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>248</v>
+        <v>205</v>
       </c>
       <c r="B53" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="C53" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
       <c r="B54" t="s">
-        <v>249</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>250</v>
+        <v>46</v>
       </c>
       <c r="D54" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>239</v>
+        <v>201</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>90</v>
+        <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>239</v>
+        <v>201</v>
       </c>
       <c r="B56" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="D56" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>239</v>
+        <v>199</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>92</v>
+        <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>239</v>
+        <v>199</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="C58" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="D58" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="B59" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="C59" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="D59" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="B60" t="s">
-        <v>251</v>
+        <v>70</v>
       </c>
       <c r="C60" t="s">
-        <v>250</v>
+        <v>46</v>
       </c>
       <c r="D60" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B61" t="s">
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="C61" t="s">
-        <v>90</v>
+        <v>213</v>
       </c>
       <c r="D61" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B62" t="s">
-        <v>103</v>
+        <v>254</v>
       </c>
       <c r="C62" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="D62" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B63" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C63" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D63" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D64" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B65" t="s">
-        <v>106</v>
+        <v>255</v>
       </c>
       <c r="C65" t="s">
-        <v>94</v>
+        <v>253</v>
       </c>
       <c r="D65" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="B66" t="s">
-        <v>252</v>
+        <v>77</v>
       </c>
       <c r="C66" t="s">
-        <v>250</v>
+        <v>73</v>
       </c>
       <c r="D66" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>214</v>
       </c>
       <c r="C67" t="s">
-        <v>90</v>
+        <v>213</v>
       </c>
       <c r="D67" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B68" t="s">
-        <v>109</v>
+        <v>256</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="D68" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B69" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="C69" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D69" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B70" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C70" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D70" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B71" t="s">
-        <v>112</v>
+        <v>257</v>
       </c>
       <c r="C71" t="s">
-        <v>94</v>
+        <v>253</v>
       </c>
       <c r="D71" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="B72" t="s">
-        <v>253</v>
+        <v>81</v>
       </c>
       <c r="C72" t="s">
-        <v>250</v>
+        <v>73</v>
       </c>
       <c r="D72" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B73" t="s">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="C73" t="s">
-        <v>90</v>
+        <v>213</v>
       </c>
       <c r="D73" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B74" t="s">
-        <v>115</v>
+        <v>258</v>
       </c>
       <c r="C74" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="D74" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B75" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="C75" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D75" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B76" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="C76" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D76" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B77" t="s">
-        <v>118</v>
+        <v>259</v>
       </c>
       <c r="C77" t="s">
-        <v>94</v>
+        <v>253</v>
       </c>
       <c r="D77" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>242</v>
+        <v>200</v>
       </c>
       <c r="B78" t="s">
-        <v>254</v>
+        <v>85</v>
       </c>
       <c r="C78" t="s">
-        <v>250</v>
+        <v>73</v>
       </c>
       <c r="D78" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B79" t="s">
-        <v>120</v>
+        <v>216</v>
       </c>
       <c r="C79" t="s">
-        <v>90</v>
+        <v>213</v>
       </c>
       <c r="D79" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B80" t="s">
-        <v>121</v>
+        <v>260</v>
       </c>
       <c r="C80" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="D80" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B81" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="C81" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D81" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B82" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="C82" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D82" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B83" t="s">
-        <v>124</v>
+        <v>261</v>
       </c>
       <c r="C83" t="s">
-        <v>94</v>
+        <v>253</v>
       </c>
       <c r="D83" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="B84" t="s">
-        <v>255</v>
+        <v>89</v>
       </c>
       <c r="C84" t="s">
-        <v>250</v>
+        <v>73</v>
       </c>
       <c r="D84" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B85" t="s">
-        <v>126</v>
+        <v>217</v>
       </c>
       <c r="C85" t="s">
+        <v>213</v>
+      </c>
+      <c r="D85" t="s">
         <v>90</v>
-      </c>
-      <c r="D85" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B86" t="s">
-        <v>127</v>
+        <v>262</v>
       </c>
       <c r="C86" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="D86" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B87" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="C87" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D87" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B88" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="C88" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D88" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B89" t="s">
-        <v>130</v>
+        <v>263</v>
       </c>
       <c r="C89" t="s">
-        <v>94</v>
+        <v>253</v>
       </c>
       <c r="D89" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="B90" t="s">
-        <v>256</v>
+        <v>93</v>
       </c>
       <c r="C90" t="s">
-        <v>250</v>
+        <v>73</v>
       </c>
       <c r="D90" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B91" t="s">
-        <v>132</v>
+        <v>218</v>
       </c>
       <c r="C91" t="s">
-        <v>90</v>
+        <v>213</v>
       </c>
       <c r="D91" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B92" t="s">
-        <v>133</v>
+        <v>264</v>
       </c>
       <c r="C92" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="D92" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B93" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D93" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B94" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="C94" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D94" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B95" t="s">
-        <v>136</v>
+        <v>265</v>
       </c>
       <c r="C95" t="s">
+        <v>253</v>
+      </c>
+      <c r="D95" t="s">
         <v>94</v>
-      </c>
-      <c r="D95" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>248</v>
+        <v>201</v>
       </c>
       <c r="B96" t="s">
-        <v>257</v>
+        <v>97</v>
       </c>
       <c r="C96" t="s">
-        <v>250</v>
+        <v>73</v>
       </c>
       <c r="D96" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B97" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="C97" t="s">
-        <v>90</v>
+        <v>213</v>
       </c>
       <c r="D97" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B98" t="s">
-        <v>139</v>
+        <v>266</v>
       </c>
       <c r="C98" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="D98" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B99" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="C99" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D99" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B100" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="C100" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D100" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B101" t="s">
-        <v>142</v>
+        <v>267</v>
       </c>
       <c r="C101" t="s">
-        <v>94</v>
+        <v>253</v>
       </c>
       <c r="D101" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>239</v>
+        <v>199</v>
       </c>
       <c r="B102" t="s">
-        <v>258</v>
+        <v>101</v>
       </c>
       <c r="C102" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="D102" t="s">
-        <v>152</v>
+        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="B103" t="s">
-        <v>259</v>
+        <v>220</v>
       </c>
       <c r="C103" t="s">
-        <v>143</v>
+        <v>213</v>
       </c>
       <c r="D103" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="B104" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="C104" t="s">
-        <v>144</v>
+        <v>252</v>
       </c>
       <c r="D104" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="B105" t="s">
-        <v>261</v>
+        <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>145</v>
+        <v>71</v>
       </c>
       <c r="D105" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="B106" t="s">
-        <v>262</v>
+        <v>104</v>
       </c>
       <c r="C106" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="D106" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="B107" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="C107" t="s">
-        <v>147</v>
+        <v>253</v>
       </c>
       <c r="D107" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="B108" t="s">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="C108" t="s">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="D108" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="B109" t="s">
-        <v>154</v>
+        <v>221</v>
       </c>
       <c r="C109" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="D109" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="B110" t="s">
-        <v>155</v>
+        <v>222</v>
       </c>
       <c r="C110" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="D110" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="B111" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="C111" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="D111" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B112" t="s">
-        <v>157</v>
+        <v>224</v>
       </c>
       <c r="C112" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="D112" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B113" t="s">
-        <v>159</v>
+        <v>225</v>
       </c>
       <c r="C113" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="D113" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B114" t="s">
-        <v>160</v>
+        <v>226</v>
       </c>
       <c r="C114" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="D114" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B115" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="C115" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="D115" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B116" t="s">
-        <v>162</v>
+        <v>117</v>
       </c>
       <c r="C116" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="D116" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B117" t="s">
-        <v>163</v>
+        <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="D117" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="B118" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
       <c r="C118" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="D118" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
       <c r="B119" t="s">
-        <v>165</v>
+        <v>120</v>
       </c>
       <c r="C119" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="D119" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
       <c r="B120" t="s">
-        <v>166</v>
+        <v>122</v>
       </c>
       <c r="C120" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="D120" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
       <c r="B121" t="s">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="C121" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="D121" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B122" t="s">
-        <v>168</v>
+        <v>124</v>
       </c>
       <c r="C122" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="D122" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B123" t="s">
-        <v>170</v>
+        <v>125</v>
       </c>
       <c r="C123" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="D123" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B124" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="C124" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="D124" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B125" t="s">
-        <v>172</v>
+        <v>127</v>
       </c>
       <c r="C125" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="D125" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B126" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="C126" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="D126" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B127" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="C127" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="D127" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B128" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="C128" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="D128" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="B129" t="s">
-        <v>176</v>
+        <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="D129" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="B130" t="s">
-        <v>177</v>
+        <v>133</v>
       </c>
       <c r="C130" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="D130" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="B131" t="s">
-        <v>178</v>
+        <v>134</v>
       </c>
       <c r="C131" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="D131" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B132" t="s">
-        <v>179</v>
+        <v>135</v>
       </c>
       <c r="C132" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="D132" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B133" t="s">
-        <v>181</v>
+        <v>136</v>
       </c>
       <c r="C133" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="D133" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B134" t="s">
-        <v>182</v>
+        <v>137</v>
       </c>
       <c r="C134" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="D134" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B135" t="s">
-        <v>183</v>
+        <v>138</v>
       </c>
       <c r="C135" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="D135" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B136" t="s">
-        <v>184</v>
+        <v>139</v>
       </c>
       <c r="C136" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="D136" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B137" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="C137" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="D137" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B138" t="s">
-        <v>186</v>
+        <v>141</v>
       </c>
       <c r="C138" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="D138" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="B139" t="s">
-        <v>187</v>
+        <v>142</v>
       </c>
       <c r="C139" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="D139" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="B140" t="s">
-        <v>188</v>
+        <v>144</v>
       </c>
       <c r="C140" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="D140" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="B141" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="C141" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="D141" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B142" t="s">
-        <v>190</v>
+        <v>146</v>
       </c>
       <c r="C142" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="D142" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B143" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="C143" t="s">
+        <v>109</v>
+      </c>
+      <c r="D143" t="s">
         <v>143</v>
-      </c>
-      <c r="D143" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B144" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="C144" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="D144" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B145" t="s">
-        <v>194</v>
+        <v>149</v>
       </c>
       <c r="C145" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="D145" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B146" t="s">
-        <v>195</v>
+        <v>150</v>
       </c>
       <c r="C146" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="D146" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B147" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
       <c r="C147" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="D147" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B148" t="s">
-        <v>197</v>
+        <v>152</v>
       </c>
       <c r="C148" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="D148" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="B149" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="C149" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="D149" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="B150" t="s">
-        <v>199</v>
+        <v>155</v>
       </c>
       <c r="C150" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="D150" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="B151" t="s">
-        <v>200</v>
+        <v>156</v>
       </c>
       <c r="C151" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="D151" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B152" t="s">
-        <v>201</v>
+        <v>157</v>
       </c>
       <c r="C152" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="D152" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B153" t="s">
-        <v>203</v>
+        <v>158</v>
       </c>
       <c r="C153" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="D153" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B154" t="s">
-        <v>204</v>
+        <v>159</v>
       </c>
       <c r="C154" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="D154" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B155" t="s">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="C155" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="D155" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B156" t="s">
-        <v>206</v>
+        <v>161</v>
       </c>
       <c r="C156" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="D156" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B157" t="s">
-        <v>207</v>
+        <v>162</v>
       </c>
       <c r="C157" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="D157" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B158" t="s">
-        <v>208</v>
+        <v>163</v>
       </c>
       <c r="C158" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="D158" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="B159" t="s">
-        <v>209</v>
+        <v>164</v>
       </c>
       <c r="C159" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="D159" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="B160" t="s">
-        <v>210</v>
+        <v>166</v>
       </c>
       <c r="C160" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="D160" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="B161" t="s">
-        <v>211</v>
+        <v>167</v>
       </c>
       <c r="C161" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="D161" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B162" t="s">
-        <v>212</v>
+        <v>168</v>
       </c>
       <c r="C162" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="D162" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B163" t="s">
-        <v>214</v>
+        <v>169</v>
       </c>
       <c r="C163" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="D163" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B164" t="s">
-        <v>215</v>
+        <v>170</v>
       </c>
       <c r="C164" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="D164" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B165" t="s">
-        <v>216</v>
+        <v>171</v>
       </c>
       <c r="C165" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="D165" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B166" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="C166" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="D166" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B167" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
       <c r="C167" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="D167" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B168" t="s">
-        <v>219</v>
+        <v>174</v>
       </c>
       <c r="C168" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="D168" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="B169" t="s">
-        <v>220</v>
+        <v>175</v>
       </c>
       <c r="C169" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="D169" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="B170" t="s">
-        <v>221</v>
+        <v>177</v>
       </c>
       <c r="C170" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="D170" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="B171" t="s">
-        <v>222</v>
+        <v>178</v>
       </c>
       <c r="C171" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="D171" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B172" t="s">
-        <v>223</v>
+        <v>179</v>
       </c>
       <c r="C172" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="D172" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B173" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="C173" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="D173" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B174" t="s">
-        <v>226</v>
+        <v>181</v>
       </c>
       <c r="C174" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="D174" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B175" t="s">
-        <v>227</v>
+        <v>182</v>
       </c>
       <c r="C175" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="D175" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B176" t="s">
-        <v>228</v>
+        <v>183</v>
       </c>
       <c r="C176" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="D176" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B177" t="s">
-        <v>229</v>
+        <v>184</v>
       </c>
       <c r="C177" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="D177" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B178" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="C178" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="D178" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="B179" t="s">
-        <v>231</v>
+        <v>186</v>
       </c>
       <c r="C179" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="D179" t="s">
-        <v>224</v>
+        <v>187</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="B180" t="s">
-        <v>232</v>
+        <v>188</v>
       </c>
       <c r="C180" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="D180" t="s">
-        <v>224</v>
+        <v>187</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="B181" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
       <c r="C181" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="D181" t="s">
-        <v>224</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>211</v>
+      </c>
+      <c r="B182" t="s">
+        <v>190</v>
+      </c>
+      <c r="C182" t="s">
+        <v>108</v>
+      </c>
+      <c r="D182" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>211</v>
+      </c>
+      <c r="B183" t="s">
+        <v>191</v>
+      </c>
+      <c r="C183" t="s">
+        <v>109</v>
+      </c>
+      <c r="D183" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>211</v>
+      </c>
+      <c r="B184" t="s">
+        <v>192</v>
+      </c>
+      <c r="C184" t="s">
+        <v>110</v>
+      </c>
+      <c r="D184" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>211</v>
+      </c>
+      <c r="B185" t="s">
+        <v>193</v>
+      </c>
+      <c r="C185" t="s">
+        <v>111</v>
+      </c>
+      <c r="D185" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>211</v>
+      </c>
+      <c r="B186" t="s">
+        <v>194</v>
+      </c>
+      <c r="C186" t="s">
+        <v>112</v>
+      </c>
+      <c r="D186" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>211</v>
+      </c>
+      <c r="B187" t="s">
+        <v>195</v>
+      </c>
+      <c r="C187" t="s">
+        <v>113</v>
+      </c>
+      <c r="D187" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>211</v>
+      </c>
+      <c r="B188" t="s">
+        <v>196</v>
+      </c>
+      <c r="C188" t="s">
+        <v>114</v>
+      </c>
+      <c r="D188" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>